<commit_message>
-Added in Helliquary Raid timers.
</commit_message>
<xml_diff>
--- a/DI_Timer_App/ResetTable.xlsx
+++ b/DI_Timer_App/ResetTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\diablo_immortal_event_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D23345-4360-46D7-A7ED-A41ACAD71B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B50DAE-D401-42FF-B888-A61483DE00D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{314A5783-AB47-4A14-A3F0-7080D14E4476}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{314A5783-AB47-4A14-A3F0-7080D14E4476}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Countdown</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Weekly Reset</t>
+  </si>
+  <si>
+    <t>Helliquary Raid</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBD3C64-1693-4C51-AB75-FB92840AA828}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +478,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>